<commit_message>
seperated game from vis
</commit_message>
<xml_diff>
--- a/utilities/filepathBuilder.xlsx
+++ b/utilities/filepathBuilder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\py\mr-game-webapp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\py\mr-game-webapp\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29CCCC5-2FD6-4CB8-853C-7940F622F0A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B7DAEE-7A0A-4899-8ADA-D0F839E76CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="-98" windowWidth="19477" windowHeight="13875" xr2:uid="{0D1D6570-FBCC-4FB8-B9DE-1CBA81988DC6}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{0D1D6570-FBCC-4FB8-B9DE-1CBA81988DC6}"/>
   </bookViews>
   <sheets>
     <sheet name="assets" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>C:\py\mr-game-webapp\audio\sounds\ships\flyby_fast_1.mp3</t>
   </si>
@@ -215,21 +215,12 @@
     <t>C:\py\mr-game-webapp\images\spaceboxes\space2.jpg</t>
   </si>
   <si>
-    <t>C:\py\mr-game-webapp\images\epicons\anxiety.png</t>
-  </si>
-  <si>
     <t>C:\py\mr-game-webapp\images\epicons\bmi.png</t>
   </si>
   <si>
     <t>C:\py\mr-game-webapp\images\epicons\caffeine.png</t>
   </si>
   <si>
-    <t>C:\py\mr-game-webapp\images\epicons\chd.png</t>
-  </si>
-  <si>
-    <t>C:\py\mr-game-webapp\images\epicons\depression.png</t>
-  </si>
-  <si>
     <t>C:\py\mr-game-webapp\images\epicons\diabetes.png</t>
   </si>
   <si>
@@ -239,42 +230,15 @@
     <t>C:\py\mr-game-webapp\images\epicons\drugs.png</t>
   </si>
   <si>
-    <t>C:\py\mr-game-webapp\images\epicons\education.png</t>
-  </si>
-  <si>
-    <t>C:\py\mr-game-webapp\images\epicons\exercise.png</t>
-  </si>
-  <si>
     <t>C:\py\mr-game-webapp\images\epicons\gaming.png</t>
   </si>
   <si>
     <t>C:\py\mr-game-webapp\images\epicons\intelligence.png</t>
   </si>
   <si>
-    <t>C:\py\mr-game-webapp\images\epicons\loneliness.png</t>
-  </si>
-  <si>
-    <t>C:\py\mr-game-webapp\images\epicons\loneliness_alt.png</t>
-  </si>
-  <si>
-    <t>C:\py\mr-game-webapp\images\epicons\notSocial1.png</t>
-  </si>
-  <si>
-    <t>C:\py\mr-game-webapp\images\epicons\notSocial2.png</t>
-  </si>
-  <si>
-    <t>C:\py\mr-game-webapp\images\epicons\ocd.png</t>
-  </si>
-  <si>
     <t>C:\py\mr-game-webapp\images\epicons\phone.png</t>
   </si>
   <si>
-    <t>C:\py\mr-game-webapp\images\epicons\shifts.png</t>
-  </si>
-  <si>
-    <t>C:\py\mr-game-webapp\images\epicons\shifts_alt.png</t>
-  </si>
-  <si>
     <t>C:\py\mr-game-webapp\images\epicons\sleep_duration.png</t>
   </si>
   <si>
@@ -284,10 +248,55 @@
     <t>C:\py\mr-game-webapp\images\epicons\smoking.png</t>
   </si>
   <si>
-    <t>C:\py\mr-game-webapp\images\epicons\social.png</t>
-  </si>
-  <si>
-    <t>C:\py\mr-game-webapp\images\epicons\wellbeing.png</t>
+    <t>C:\py\mr-game-webapp\images\epicons\chd_alt.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\education_schoolYears.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\education_schoolYears_alt.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\eveningness.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\exercise_bike.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\intelligence_alt.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\mh_anxiety2.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\mh_depression2.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\mh_ocd2.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\social_chatBubble.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\social_chatBubble_alt.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\social_loneliness.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\social_loneliness_alt.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\social_notChatting.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\wellbeing2_alt.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\work_nightShifts.png</t>
+  </si>
+  <si>
+    <t>C:\py\mr-game-webapp\images\epicons\work_nightShifts_alt.png</t>
   </si>
 </sst>
 </file>
@@ -647,28 +656,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C9BDCDD-2004-4A19-AD4C-2E7B825EE2D8}">
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B51" workbookViewId="0">
-      <selection activeCell="F77" sqref="F51:F77"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51:F79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -693,7 +702,7 @@
         <v>'audio\sounds\ships\flyby_fast_1.mp3',</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -718,7 +727,7 @@
         <v>'audio\sounds\ships\flyby_fast_2.mp3',</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -743,7 +752,7 @@
         <v>'audio\sounds\ships\flyby_med_1.mp3',</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -768,7 +777,7 @@
         <v>'audio\sounds\ships\flyby_med_2.mp3',</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -793,7 +802,7 @@
         <v>'audio\sounds\ships\flyby_slow_1.wav',</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -818,7 +827,7 @@
         <v>'audio\sounds\ships\flyby_veryfast_1.wav',</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -843,12 +852,12 @@
         <v>'audio\sounds\ships\flyby_veryslow_1.mp3',</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -873,7 +882,7 @@
         <v>'audio\music\01_infinity_awaits_us.mp3',</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -898,7 +907,7 @@
         <v>'audio\music\02_miniboss.mp3',</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -923,7 +932,7 @@
         <v>'audio\music\03_imagine.mp3',</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -948,7 +957,7 @@
         <v>'audio\music\04_artificial_serenity.mp3',</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -973,7 +982,7 @@
         <v>'audio\music\05_castles_of_ice.mp3',</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -998,7 +1007,7 @@
         <v>'audio\music\06_tetanus.mp3',</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1023,7 +1032,7 @@
         <v>'audio\music\07_flora.mp3',</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1048,7 +1057,7 @@
         <v>'audio\music\08_glades.mp3',</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1073,7 +1082,7 @@
         <v>'audio\music\09_village.mp3',</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1098,7 +1107,7 @@
         <v>'audio\music\10_cascade.mp3',</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1123,7 +1132,7 @@
         <v>'audio\music\11_claustrophobia.mp3',</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1148,7 +1157,7 @@
         <v>'audio\music\12_boss.mp3',</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1173,7 +1182,7 @@
         <v>'audio\music\13_spheres.mp3',</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1198,7 +1207,7 @@
         <v>'audio\music\14_skeletons.mp3',</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1223,7 +1232,7 @@
         <v>'audio\music\15_men_of_stone.mp3',</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1248,7 +1257,7 @@
         <v>'audio\music\16_deaths_embrace.mp3',</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1273,12 +1282,12 @@
         <v>'audio\music\17_omnia_peratus.mp3',</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1303,7 +1312,7 @@
         <v>'images\ships\rocket_comet.png',</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -1316,7 +1325,7 @@
         <v>'images\ships\rocket_emperor.png',</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1329,7 +1338,7 @@
         <v>'images\ships\rocket_explorer1.png',</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1342,7 +1351,7 @@
         <v>'images\ships\rocket_explorer2.png',</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -1355,7 +1364,7 @@
         <v>'images\ships\rocket_mule.png',</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -1368,7 +1377,7 @@
         <v>'images\ships\rocket_prestige.png',</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -1381,12 +1390,12 @@
         <v>'images\ships\rocket_whale.png',</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1411,7 +1420,7 @@
         <v>'images\planets\earth.png',</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1436,7 +1445,7 @@
         <v>'images\planets\newearth.png',</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1461,7 +1470,7 @@
         <v>'images\planets\earth1.png',</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1486,7 +1495,7 @@
         <v>'images\planets\earth2.png',</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1511,7 +1520,7 @@
         <v>'images\planets\earth3.png',</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1536,7 +1545,7 @@
         <v>'images\planets\earth4.png',</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1561,7 +1570,7 @@
         <v>'images\planets\jupiter.png',</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1586,7 +1595,7 @@
         <v>'images\planets\mars.png',</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1611,7 +1620,7 @@
         <v>'images\planets\mercury.png',</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1636,7 +1645,7 @@
         <v>'images\planets\neptune.png',</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1661,7 +1670,7 @@
         <v>'images\planets\saturn.png',</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1686,7 +1695,7 @@
         <v>'images\planets\saturn2.png',</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1711,7 +1720,7 @@
         <v>'images\planets\uranus.png',</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1736,887 +1745,937 @@
         <v>'images\planets\venus.png',</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" ref="B51" si="19">RIGHT(A51,LEN(A51)-33)</f>
-        <v>ns\sleep.png</v>
+        <v>ns\bmi.png</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" ref="C51" si="20">LEFT(RIGHT(A51,LEN(A51)-33),LEN(A51)-37)</f>
-        <v>ns\sleep</v>
+        <v>ns\bmi</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" ref="D51" si="21">"'"&amp;C51&amp;"',"</f>
-        <v>'ns\sleep',</v>
+        <v>'ns\bmi',</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" ref="E51" si="22">RIGHT(A51,LEN(A51)-21)</f>
-        <v>images\epicons\sleep.png</v>
+        <v>images\epicons\bmi.png</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="4"/>
-        <v>'images\epicons\sleep.png',</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\bmi.png',</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B52" t="str">
-        <f t="shared" ref="B52:B77" si="23">RIGHT(A52,LEN(A52)-33)</f>
-        <v>ns\anxiety.png</v>
+        <f t="shared" ref="B52:B79" si="23">RIGHT(A52,LEN(A52)-33)</f>
+        <v>ns\caffeine.png</v>
       </c>
       <c r="C52" t="str">
-        <f t="shared" ref="C52:C77" si="24">LEFT(RIGHT(A52,LEN(A52)-33),LEN(A52)-37)</f>
-        <v>ns\anxiety</v>
+        <f t="shared" ref="C52:C79" si="24">LEFT(RIGHT(A52,LEN(A52)-33),LEN(A52)-37)</f>
+        <v>ns\caffeine</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" ref="D52:D77" si="25">"'"&amp;C52&amp;"',"</f>
-        <v>'ns\anxiety',</v>
+        <f t="shared" ref="D52:D79" si="25">"'"&amp;C52&amp;"',"</f>
+        <v>'ns\caffeine',</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" ref="E52:E77" si="26">RIGHT(A52,LEN(A52)-21)</f>
-        <v>images\epicons\anxiety.png</v>
+        <f t="shared" ref="E52:E79" si="26">RIGHT(A52,LEN(A52)-21)</f>
+        <v>images\epicons\caffeine.png</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" ref="F52:F77" si="27">"'"&amp;E52&amp;"',"</f>
-        <v>'images\epicons\anxiety.png',</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+        <f t="shared" ref="F52:F79" si="27">"'"&amp;E52&amp;"',"</f>
+        <v>'images\epicons\caffeine.png',</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="23"/>
-        <v>ns\bmi.png</v>
+        <v>ns\chd_alt.png</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="24"/>
-        <v>ns\bmi</v>
+        <v>ns\chd_alt</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\bmi',</v>
+        <v>'ns\chd_alt',</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\bmi.png</v>
+        <v>images\epicons\chd_alt.png</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\bmi.png',</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\chd_alt.png',</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>62</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="23"/>
-        <v>ns\caffeine.png</v>
+        <v>ns\diabetes.png</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="24"/>
-        <v>ns\caffeine</v>
+        <v>ns\diabetes</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\caffeine',</v>
+        <v>'ns\diabetes',</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\caffeine.png</v>
+        <v>images\epicons\diabetes.png</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\caffeine.png',</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\diabetes.png',</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>63</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="23"/>
-        <v>ns\chd.png</v>
+        <v>ns\drinking.png</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="24"/>
-        <v>ns\chd</v>
+        <v>ns\drinking</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\chd',</v>
+        <v>'ns\drinking',</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\chd.png</v>
+        <v>images\epicons\drinking.png</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\chd.png',</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\drinking.png',</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>64</v>
       </c>
       <c r="B56" t="str">
         <f t="shared" si="23"/>
-        <v>ns\depression.png</v>
+        <v>ns\drugs.png</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="24"/>
-        <v>ns\depression</v>
+        <v>ns\drugs</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\depression',</v>
+        <v>'ns\drugs',</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\depression.png</v>
+        <v>images\epicons\drugs.png</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\depression.png',</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\drugs.png',</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="23"/>
-        <v>ns\diabetes.png</v>
+        <v>ns\education_schoolYears.png</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="24"/>
-        <v>ns\diabetes</v>
+        <v>ns\education_schoolYears</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\diabetes',</v>
+        <v>'ns\education_schoolYears',</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\diabetes.png</v>
+        <v>images\epicons\education_schoolYears.png</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\diabetes.png',</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\education_schoolYears.png',</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="23"/>
-        <v>ns\drinking.png</v>
+        <v>ns\education_schoolYears_alt.png</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="24"/>
-        <v>ns\drinking</v>
+        <v>ns\education_schoolYears_alt</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\drinking',</v>
+        <v>'ns\education_schoolYears_alt',</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\drinking.png</v>
+        <v>images\epicons\education_schoolYears_alt.png</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\drinking.png',</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\education_schoolYears_alt.png',</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="23"/>
-        <v>ns\drugs.png</v>
+        <v>ns\eveningness.png</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="24"/>
-        <v>ns\drugs</v>
+        <v>ns\eveningness</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\drugs',</v>
+        <v>'ns\eveningness',</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\drugs.png</v>
+        <v>images\epicons\eveningness.png</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\drugs.png',</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\eveningness.png',</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="23"/>
-        <v>ns\education.png</v>
+        <v>ns\exercise_bike.png</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="24"/>
-        <v>ns\education</v>
+        <v>ns\exercise_bike</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\education',</v>
+        <v>'ns\exercise_bike',</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\education.png</v>
+        <v>images\epicons\exercise_bike.png</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\education.png',</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\exercise_bike.png',</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B61" t="str">
         <f t="shared" si="23"/>
-        <v>ns\exercise.png</v>
+        <v>ns\gaming.png</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="24"/>
-        <v>ns\exercise</v>
+        <v>ns\gaming</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\exercise',</v>
+        <v>'ns\gaming',</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\exercise.png</v>
+        <v>images\epicons\gaming.png</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\exercise.png',</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\gaming.png',</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="23"/>
-        <v>ns\gaming.png</v>
+        <v>ns\intelligence.png</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="24"/>
-        <v>ns\gaming</v>
+        <v>ns\intelligence</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\gaming',</v>
+        <v>'ns\intelligence',</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\gaming.png</v>
+        <v>images\epicons\intelligence.png</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\gaming.png',</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\intelligence.png',</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" si="23"/>
-        <v>ns\intelligence.png</v>
+        <v>ns\intelligence_alt.png</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="24"/>
-        <v>ns\intelligence</v>
+        <v>ns\intelligence_alt</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\intelligence',</v>
+        <v>'ns\intelligence_alt',</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\intelligence.png</v>
+        <v>images\epicons\intelligence_alt.png</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\intelligence.png',</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\intelligence_alt.png',</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B64" t="str">
         <f t="shared" si="23"/>
-        <v>ns\loneliness.png</v>
+        <v>ns\mh_anxiety2.png</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="24"/>
-        <v>ns\loneliness</v>
+        <v>ns\mh_anxiety2</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\loneliness',</v>
+        <v>'ns\mh_anxiety2',</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\loneliness.png</v>
+        <v>images\epicons\mh_anxiety2.png</v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\loneliness.png',</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\mh_anxiety2.png',</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B65" t="str">
         <f t="shared" si="23"/>
-        <v>ns\loneliness_alt.png</v>
+        <v>ns\mh_depression2.png</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="24"/>
-        <v>ns\loneliness_alt</v>
+        <v>ns\mh_depression2</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\loneliness_alt',</v>
+        <v>'ns\mh_depression2',</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\loneliness_alt.png</v>
+        <v>images\epicons\mh_depression2.png</v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\loneliness_alt.png',</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\mh_depression2.png',</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B66" t="str">
         <f t="shared" si="23"/>
-        <v>ns\notSocial1.png</v>
+        <v>ns\mh_ocd2.png</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="24"/>
-        <v>ns\notSocial1</v>
+        <v>ns\mh_ocd2</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\notSocial1',</v>
+        <v>'ns\mh_ocd2',</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\notSocial1.png</v>
+        <v>images\epicons\mh_ocd2.png</v>
       </c>
       <c r="F66" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\notSocial1.png',</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\mh_ocd2.png',</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B67" t="str">
         <f t="shared" si="23"/>
-        <v>ns\notSocial2.png</v>
+        <v>ns\phone.png</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="24"/>
-        <v>ns\notSocial2</v>
+        <v>ns\phone</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\notSocial2',</v>
+        <v>'ns\phone',</v>
       </c>
       <c r="E67" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\notSocial2.png</v>
+        <v>images\epicons\phone.png</v>
       </c>
       <c r="F67" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\notSocial2.png',</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\phone.png',</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="23"/>
-        <v>ns\ocd.png</v>
+        <v>ns\sleep.png</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="24"/>
-        <v>ns\ocd</v>
+        <v>ns\sleep</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\ocd',</v>
+        <v>'ns\sleep',</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\ocd.png</v>
+        <v>images\epicons\sleep.png</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\ocd.png',</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\sleep.png',</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="23"/>
-        <v>ns\phone.png</v>
+        <v>ns\sleep_duration.png</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="24"/>
-        <v>ns\phone</v>
+        <v>ns\sleep_duration</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\phone',</v>
+        <v>'ns\sleep_duration',</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\phone.png</v>
+        <v>images\epicons\sleep_duration.png</v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\phone.png',</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\sleep_duration.png',</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B70" t="str">
         <f t="shared" si="23"/>
-        <v>ns\shifts.png</v>
+        <v>ns\sleep_insomnia.png</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="24"/>
-        <v>ns\shifts</v>
+        <v>ns\sleep_insomnia</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\shifts',</v>
+        <v>'ns\sleep_insomnia',</v>
       </c>
       <c r="E70" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\shifts.png</v>
+        <v>images\epicons\sleep_insomnia.png</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\shifts.png',</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\sleep_insomnia.png',</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B71" t="str">
         <f t="shared" si="23"/>
-        <v>ns\shifts_alt.png</v>
+        <v>ns\smoking.png</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="24"/>
-        <v>ns\shifts_alt</v>
+        <v>ns\smoking</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\shifts_alt',</v>
+        <v>'ns\smoking',</v>
       </c>
       <c r="E71" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\shifts_alt.png</v>
+        <v>images\epicons\smoking.png</v>
       </c>
       <c r="F71" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\shifts_alt.png',</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\smoking.png',</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="B72" t="str">
         <f t="shared" si="23"/>
-        <v>ns\sleep.png</v>
+        <v>ns\social_chatBubble.png</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="24"/>
-        <v>ns\sleep</v>
+        <v>ns\social_chatBubble</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\sleep',</v>
+        <v>'ns\social_chatBubble',</v>
       </c>
       <c r="E72" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\sleep.png</v>
+        <v>images\epicons\social_chatBubble.png</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\sleep.png',</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\social_chatBubble.png',</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" si="23"/>
-        <v>ns\sleep_duration.png</v>
+        <v>ns\social_chatBubble_alt.png</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="24"/>
-        <v>ns\sleep_duration</v>
+        <v>ns\social_chatBubble_alt</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\sleep_duration',</v>
+        <v>'ns\social_chatBubble_alt',</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\sleep_duration.png</v>
+        <v>images\epicons\social_chatBubble_alt.png</v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\sleep_duration.png',</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\social_chatBubble_alt.png',</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="23"/>
-        <v>ns\sleep_insomnia.png</v>
+        <v>ns\social_loneliness.png</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="24"/>
-        <v>ns\sleep_insomnia</v>
+        <v>ns\social_loneliness</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\sleep_insomnia',</v>
+        <v>'ns\social_loneliness',</v>
       </c>
       <c r="E74" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\sleep_insomnia.png</v>
+        <v>images\epicons\social_loneliness.png</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\sleep_insomnia.png',</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\social_loneliness.png',</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="23"/>
-        <v>ns\smoking.png</v>
+        <v>ns\social_loneliness_alt.png</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="24"/>
-        <v>ns\smoking</v>
+        <v>ns\social_loneliness_alt</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\smoking',</v>
+        <v>'ns\social_loneliness_alt',</v>
       </c>
       <c r="E75" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\smoking.png</v>
+        <v>images\epicons\social_loneliness_alt.png</v>
       </c>
       <c r="F75" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\smoking.png',</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\social_loneliness_alt.png',</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="23"/>
-        <v>ns\social.png</v>
+        <v>ns\social_notChatting.png</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="24"/>
-        <v>ns\social</v>
+        <v>ns\social_notChatting</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\social',</v>
+        <v>'ns\social_notChatting',</v>
       </c>
       <c r="E76" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\social.png</v>
+        <v>images\epicons\social_notChatting.png</v>
       </c>
       <c r="F76" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\social.png',</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+        <v>'images\epicons\social_notChatting.png',</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="23"/>
-        <v>ns\wellbeing.png</v>
+        <v>ns\wellbeing2_alt.png</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="24"/>
-        <v>ns\wellbeing</v>
+        <v>ns\wellbeing2_alt</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="25"/>
-        <v>'ns\wellbeing',</v>
+        <v>'ns\wellbeing2_alt',</v>
       </c>
       <c r="E77" t="str">
         <f t="shared" si="26"/>
-        <v>images\epicons\wellbeing.png</v>
+        <v>images\epicons\wellbeing2_alt.png</v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="27"/>
-        <v>'images\epicons\wellbeing.png',</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A78" s="1" t="s">
+        <v>'images\epicons\wellbeing2_alt.png',</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" t="str">
+        <f t="shared" si="23"/>
+        <v>ns\work_nightShifts.png</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="24"/>
+        <v>ns\work_nightShifts</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="25"/>
+        <v>'ns\work_nightShifts',</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="26"/>
+        <v>images\epicons\work_nightShifts.png</v>
+      </c>
+      <c r="F78" t="str">
+        <f t="shared" si="27"/>
+        <v>'images\epicons\work_nightShifts.png',</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="23"/>
+        <v>ns\work_nightShifts_alt.png</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="24"/>
+        <v>ns\work_nightShifts_alt</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="25"/>
+        <v>'ns\work_nightShifts_alt',</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="26"/>
+        <v>images\epicons\work_nightShifts_alt.png</v>
+      </c>
+      <c r="F79" t="str">
+        <f t="shared" si="27"/>
+        <v>'images\epicons\work_nightShifts_alt.png',</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>52</v>
       </c>
-      <c r="B79" t="str">
-        <f t="shared" ref="B79" si="28">RIGHT(A79,LEN(A79)-33)</f>
+      <c r="B88" t="str">
+        <f t="shared" ref="B88" si="28">RIGHT(A88,LEN(A88)-33)</f>
         <v>boxes\1.jpg</v>
       </c>
-      <c r="C79" t="str">
-        <f t="shared" ref="C79" si="29">LEFT(RIGHT(A79,LEN(A79)-33),LEN(A79)-37)</f>
+      <c r="C88" t="str">
+        <f t="shared" ref="C88" si="29">LEFT(RIGHT(A88,LEN(A88)-33),LEN(A88)-37)</f>
         <v>boxes\1</v>
       </c>
-      <c r="D79" t="str">
-        <f t="shared" ref="D79" si="30">"'"&amp;C79&amp;"',"</f>
+      <c r="D88" t="str">
+        <f t="shared" ref="D88" si="30">"'"&amp;C88&amp;"',"</f>
         <v>'boxes\1',</v>
       </c>
-      <c r="E79" t="str">
-        <f t="shared" ref="E79" si="31">RIGHT(A79,LEN(A79)-21)</f>
+      <c r="E88" t="str">
+        <f t="shared" ref="E88" si="31">RIGHT(A88,LEN(A88)-21)</f>
         <v>images\spaceboxes\1.jpg</v>
       </c>
-      <c r="F79" t="str">
-        <f t="shared" ref="F79" si="32">"'"&amp;E79&amp;"',"</f>
+      <c r="F88" t="str">
+        <f t="shared" ref="F88" si="32">"'"&amp;E88&amp;"',"</f>
         <v>'images\spaceboxes\1.jpg',</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>53</v>
       </c>
-      <c r="B80" t="str">
-        <f t="shared" ref="B80:B86" si="33">RIGHT(A80,LEN(A80)-33)</f>
+      <c r="B89" t="str">
+        <f t="shared" ref="B89:B95" si="33">RIGHT(A89,LEN(A89)-33)</f>
         <v>boxes\2.jpg</v>
       </c>
-      <c r="C80" t="str">
-        <f t="shared" ref="C80:C86" si="34">LEFT(RIGHT(A80,LEN(A80)-33),LEN(A80)-37)</f>
+      <c r="C89" t="str">
+        <f t="shared" ref="C89:C95" si="34">LEFT(RIGHT(A89,LEN(A89)-33),LEN(A89)-37)</f>
         <v>boxes\2</v>
       </c>
-      <c r="D80" t="str">
-        <f t="shared" ref="D80:D86" si="35">"'"&amp;C80&amp;"',"</f>
+      <c r="D89" t="str">
+        <f t="shared" ref="D89:D95" si="35">"'"&amp;C89&amp;"',"</f>
         <v>'boxes\2',</v>
       </c>
-      <c r="E80" t="str">
-        <f t="shared" ref="E80:E86" si="36">RIGHT(A80,LEN(A80)-21)</f>
+      <c r="E89" t="str">
+        <f t="shared" ref="E89:E95" si="36">RIGHT(A89,LEN(A89)-21)</f>
         <v>images\spaceboxes\2.jpg</v>
       </c>
-      <c r="F80" t="str">
-        <f t="shared" ref="F80:F86" si="37">"'"&amp;E80&amp;"',"</f>
+      <c r="F89" t="str">
+        <f t="shared" ref="F89:F95" si="37">"'"&amp;E89&amp;"',"</f>
         <v>'images\spaceboxes\2.jpg',</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>54</v>
       </c>
-      <c r="B81" t="str">
+      <c r="B90" t="str">
         <f t="shared" si="33"/>
         <v>boxes\3.jpg</v>
       </c>
-      <c r="C81" t="str">
+      <c r="C90" t="str">
         <f t="shared" si="34"/>
         <v>boxes\3</v>
       </c>
-      <c r="D81" t="str">
+      <c r="D90" t="str">
         <f t="shared" si="35"/>
         <v>'boxes\3',</v>
       </c>
-      <c r="E81" t="str">
+      <c r="E90" t="str">
         <f t="shared" si="36"/>
         <v>images\spaceboxes\3.jpg</v>
       </c>
-      <c r="F81" t="str">
+      <c r="F90" t="str">
         <f t="shared" si="37"/>
         <v>'images\spaceboxes\3.jpg',</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>55</v>
       </c>
-      <c r="B82" t="str">
+      <c r="B91" t="str">
         <f t="shared" si="33"/>
         <v>boxes\4.jpg</v>
       </c>
-      <c r="C82" t="str">
+      <c r="C91" t="str">
         <f t="shared" si="34"/>
         <v>boxes\4</v>
       </c>
-      <c r="D82" t="str">
+      <c r="D91" t="str">
         <f t="shared" si="35"/>
         <v>'boxes\4',</v>
       </c>
-      <c r="E82" t="str">
+      <c r="E91" t="str">
         <f t="shared" si="36"/>
         <v>images\spaceboxes\4.jpg</v>
       </c>
-      <c r="F82" t="str">
+      <c r="F91" t="str">
         <f t="shared" si="37"/>
         <v>'images\spaceboxes\4.jpg',</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>56</v>
       </c>
-      <c r="B83" t="str">
+      <c r="B92" t="str">
         <f t="shared" si="33"/>
         <v>boxes\5.jpg</v>
       </c>
-      <c r="C83" t="str">
+      <c r="C92" t="str">
         <f t="shared" si="34"/>
         <v>boxes\5</v>
       </c>
-      <c r="D83" t="str">
+      <c r="D92" t="str">
         <f t="shared" si="35"/>
         <v>'boxes\5',</v>
       </c>
-      <c r="E83" t="str">
+      <c r="E92" t="str">
         <f t="shared" si="36"/>
         <v>images\spaceboxes\5.jpg</v>
       </c>
-      <c r="F83" t="str">
+      <c r="F92" t="str">
         <f t="shared" si="37"/>
         <v>'images\spaceboxes\5.jpg',</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>57</v>
       </c>
-      <c r="B84" t="str">
+      <c r="B93" t="str">
         <f t="shared" si="33"/>
         <v>boxes\6.jpg</v>
       </c>
-      <c r="C84" t="str">
+      <c r="C93" t="str">
         <f t="shared" si="34"/>
         <v>boxes\6</v>
       </c>
-      <c r="D84" t="str">
+      <c r="D93" t="str">
         <f t="shared" si="35"/>
         <v>'boxes\6',</v>
       </c>
-      <c r="E84" t="str">
+      <c r="E93" t="str">
         <f t="shared" si="36"/>
         <v>images\spaceboxes\6.jpg</v>
       </c>
-      <c r="F84" t="str">
+      <c r="F93" t="str">
         <f t="shared" si="37"/>
         <v>'images\spaceboxes\6.jpg',</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A85" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>58</v>
       </c>
-      <c r="B85" t="str">
+      <c r="B94" t="str">
         <f t="shared" si="33"/>
         <v>boxes\7.jpg</v>
       </c>
-      <c r="C85" t="str">
+      <c r="C94" t="str">
         <f t="shared" si="34"/>
         <v>boxes\7</v>
       </c>
-      <c r="D85" t="str">
+      <c r="D94" t="str">
         <f t="shared" si="35"/>
         <v>'boxes\7',</v>
       </c>
-      <c r="E85" t="str">
+      <c r="E94" t="str">
         <f t="shared" si="36"/>
         <v>images\spaceboxes\7.jpg</v>
       </c>
-      <c r="F85" t="str">
+      <c r="F94" t="str">
         <f t="shared" si="37"/>
         <v>'images\spaceboxes\7.jpg',</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A86" t="s">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>59</v>
       </c>
-      <c r="B86" t="str">
+      <c r="B95" t="str">
         <f t="shared" si="33"/>
         <v>boxes\space2.jpg</v>
       </c>
-      <c r="C86" t="str">
+      <c r="C95" t="str">
         <f t="shared" si="34"/>
         <v>boxes\space2</v>
       </c>
-      <c r="D86" t="str">
+      <c r="D95" t="str">
         <f t="shared" si="35"/>
         <v>'boxes\space2',</v>
       </c>
-      <c r="E86" t="str">
+      <c r="E95" t="str">
         <f t="shared" si="36"/>
         <v>images\spaceboxes\space2.jpg</v>
       </c>
-      <c r="F86" t="str">
+      <c r="F95" t="str">
         <f t="shared" si="37"/>
         <v>'images\spaceboxes\space2.jpg',</v>
       </c>

</xml_diff>